<commit_message>
added sentiment analysis to report
still need to add number of positive negative and neutral
</commit_message>
<xml_diff>
--- a/Data_Report.xlsx
+++ b/Data_Report.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Logan/Documents/GitHub/CS491-BoxOffice/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Shawn/CS491-BoxOffice/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{286E4D9F-93B5-F848-93E5-84FB9C1F301D}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DE588CB-63BF-6648-90EB-31FA658BEF72}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12380" yWindow="440" windowWidth="25520" windowHeight="28360" xr2:uid="{B4E7339E-50A7-7345-85C7-648E0B2AFFAF}"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="13620" windowHeight="14340" xr2:uid="{B4E7339E-50A7-7345-85C7-648E0B2AFFAF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Movie Title</t>
   </si>
@@ -121,6 +121,9 @@
   </si>
   <si>
     <t>Total Attention</t>
+  </si>
+  <si>
+    <t>Sentiment Analysis</t>
   </si>
 </sst>
 </file>
@@ -206,7 +209,42 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="16">
+  <dxfs count="17">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.000"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="m/d/yyyy;@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="m/d/yyyy;@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="m/d/yyyy;@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -246,38 +284,6 @@
           <bgColor theme="4" tint="0.59999389629810485"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="0.000"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="m/d/yyyy;@"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="m/d/yyyy;@"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="m/d/yyyy;@"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -321,37 +327,38 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{566361E6-17D2-F04F-B2A2-701BACF21D4F}" name="Table2" displayName="Table2" ref="A1:Q16" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
-  <autoFilter ref="A1:Q16" xr:uid="{977ACCF2-D6AF-1F4D-9C8E-67F2B9073DBF}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{566361E6-17D2-F04F-B2A2-701BACF21D4F}" name="Table2" displayName="Table2" ref="A1:R16" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
+  <autoFilter ref="A1:R16" xr:uid="{977ACCF2-D6AF-1F4D-9C8E-67F2B9073DBF}"/>
   <sortState ref="A2:Q16">
     <sortCondition descending="1" ref="F1:F16"/>
   </sortState>
-  <tableColumns count="17">
-    <tableColumn id="1" xr3:uid="{E4CD3544-483B-DF4F-A8C9-8334B889ACE4}" name="Movie Title" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{BB3EFAD4-0E09-F140-848C-98D719828F82}" name="Total Tweets" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{92C49452-8A3A-8842-8631-089B162924F0}" name="Likes" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{AD276103-5716-3B43-B6C8-8D949AA97202}" name="Retweets" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{AA75EECD-212D-BD41-9C48-C3C1A08F0941}" name="Replies" dataDxfId="1"/>
-    <tableColumn id="18" xr3:uid="{76B65A6B-8381-9442-8554-32B37C575EB5}" name="Total Attention" dataDxfId="0">
+  <tableColumns count="18">
+    <tableColumn id="1" xr3:uid="{E4CD3544-483B-DF4F-A8C9-8334B889ACE4}" name="Movie Title" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{BB3EFAD4-0E09-F140-848C-98D719828F82}" name="Total Tweets" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{92C49452-8A3A-8842-8631-089B162924F0}" name="Likes" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{AD276103-5716-3B43-B6C8-8D949AA97202}" name="Retweets" dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{AA75EECD-212D-BD41-9C48-C3C1A08F0941}" name="Replies" dataDxfId="10"/>
+    <tableColumn id="18" xr3:uid="{76B65A6B-8381-9442-8554-32B37C575EB5}" name="Total Attention" dataDxfId="9">
       <calculatedColumnFormula>SUM(Table2[[#This Row],[Total Tweets]:[Replies]])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{9223458C-5ED8-3849-AA94-94576A5BF092}" name="Positive"/>
     <tableColumn id="7" xr3:uid="{DEF0B644-D2D5-1E40-834A-4535773A529A}" name="Negative"/>
     <tableColumn id="8" xr3:uid="{A82D5766-72E4-0441-B63C-DF714B35673A}" name="Neutral"/>
-    <tableColumn id="9" xr3:uid="{E745E2B8-7D49-A040-8802-3CEDBEB430DF}" name="Release Date" dataDxfId="13"/>
-    <tableColumn id="10" xr3:uid="{F67DD7E8-AB5C-824C-8812-42D2B8DC891F}" name="Data Scrape Start" dataDxfId="12">
+    <tableColumn id="9" xr3:uid="{E745E2B8-7D49-A040-8802-3CEDBEB430DF}" name="Release Date" dataDxfId="8"/>
+    <tableColumn id="10" xr3:uid="{F67DD7E8-AB5C-824C-8812-42D2B8DC891F}" name="Data Scrape Start" dataDxfId="7">
       <calculatedColumnFormula>J2-5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{BFB3861C-0060-4D4E-B8CE-ADE8871979F4}" name="Data Scrape End" dataDxfId="11">
+    <tableColumn id="11" xr3:uid="{BFB3861C-0060-4D4E-B8CE-ADE8871979F4}" name="Data Scrape End" dataDxfId="6">
       <calculatedColumnFormula>J2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{B8018AB7-FF15-C04A-A4DB-8C4612CED9D9}" name="IMDB" dataDxfId="10"/>
-    <tableColumn id="13" xr3:uid="{9BBFE118-814E-F343-A9AC-AB50B6206221}" name="Rotten Tomatoes" dataDxfId="9"/>
-    <tableColumn id="14" xr3:uid="{936BFE96-DD47-9B4D-9367-1EE99BB5465A}" name="Movie Budget" dataDxfId="8"/>
-    <tableColumn id="15" xr3:uid="{E83FF061-27B7-C84E-8DFD-65091A59DDE5}" name="Movie Earnings" dataDxfId="7"/>
-    <tableColumn id="16" xr3:uid="{6F8934A3-5EF3-A54E-B767-90F815BBFDC5}" name="Ratio" dataDxfId="6">
+    <tableColumn id="12" xr3:uid="{B8018AB7-FF15-C04A-A4DB-8C4612CED9D9}" name="IMDB" dataDxfId="5"/>
+    <tableColumn id="13" xr3:uid="{9BBFE118-814E-F343-A9AC-AB50B6206221}" name="Rotten Tomatoes" dataDxfId="4"/>
+    <tableColumn id="14" xr3:uid="{936BFE96-DD47-9B4D-9367-1EE99BB5465A}" name="Movie Budget" dataDxfId="3"/>
+    <tableColumn id="15" xr3:uid="{E83FF061-27B7-C84E-8DFD-65091A59DDE5}" name="Movie Earnings" dataDxfId="2"/>
+    <tableColumn id="16" xr3:uid="{6F8934A3-5EF3-A54E-B767-90F815BBFDC5}" name="Ratio" dataDxfId="1">
       <calculatedColumnFormula>O2/P2</calculatedColumnFormula>
     </tableColumn>
+    <tableColumn id="17" xr3:uid="{67442503-5FA6-7243-86D7-290816640E7A}" name="Sentiment Analysis" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -654,20 +661,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78DA0962-6B61-9141-A37A-CE3EA596FE55}">
-  <dimension ref="A1:Q16"/>
+  <dimension ref="A1:R16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D19" sqref="D19"/>
+      <pane xSplit="1" topLeftCell="Q1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="R16" sqref="R16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="28.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="17" width="20.83203125" customWidth="1"/>
+    <col min="18" max="18" width="31.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -719,8 +727,11 @@
       <c r="Q1" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="R1" s="1" t="s">
+        <v>32</v>
+      </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>22</v>
       </c>
@@ -744,11 +755,11 @@
         <v>42790</v>
       </c>
       <c r="K2" s="3">
-        <f>J2-5</f>
+        <f t="shared" ref="K2:K16" si="0">J2-5</f>
         <v>42785</v>
       </c>
       <c r="L2" s="3">
-        <f>J2</f>
+        <f t="shared" ref="L2:L16" si="1">J2</f>
         <v>42790</v>
       </c>
       <c r="M2" s="6">
@@ -764,11 +775,14 @@
         <v>176040665</v>
       </c>
       <c r="Q2" s="7">
-        <f>O2/P2</f>
+        <f t="shared" ref="Q2:Q16" si="2">O2/P2</f>
         <v>2.5562275625350541E-2</v>
       </c>
+      <c r="R2" s="5">
+        <v>9.1803607647199997E-2</v>
+      </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
@@ -792,11 +806,11 @@
         <v>43147</v>
       </c>
       <c r="K3" s="3">
-        <f>J3-5</f>
+        <f t="shared" si="0"/>
         <v>43142</v>
       </c>
       <c r="L3" s="3">
-        <f>J3</f>
+        <f t="shared" si="1"/>
         <v>43147</v>
       </c>
       <c r="M3" s="6">
@@ -812,11 +826,14 @@
         <v>679797522</v>
       </c>
       <c r="Q3" s="7">
-        <f>O3/P3</f>
+        <f t="shared" si="2"/>
         <v>0.29420525013328896</v>
       </c>
+      <c r="R3" s="5">
+        <v>3.8066645660800001E-3</v>
+      </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -840,11 +857,11 @@
         <v>42888</v>
       </c>
       <c r="K4" s="3">
-        <f>J4-5</f>
+        <f t="shared" si="0"/>
         <v>42883</v>
       </c>
       <c r="L4" s="3">
-        <f>J4</f>
+        <f t="shared" si="1"/>
         <v>42888</v>
       </c>
       <c r="M4" s="6">
@@ -860,11 +877,14 @@
         <v>412563408</v>
       </c>
       <c r="Q4" s="7">
-        <f>O4/P4</f>
+        <f t="shared" si="2"/>
         <v>0.36115660553201556</v>
       </c>
+      <c r="R4" s="5">
+        <v>0.112327180368</v>
+      </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>18</v>
       </c>
@@ -888,11 +908,11 @@
         <v>43084</v>
       </c>
       <c r="K5" s="3">
-        <f>J5-5</f>
+        <f t="shared" si="0"/>
         <v>43079</v>
       </c>
       <c r="L5" s="3">
-        <f>J5</f>
+        <f t="shared" si="1"/>
         <v>43084</v>
       </c>
       <c r="M5" s="6">
@@ -908,11 +928,14 @@
         <v>620174750</v>
       </c>
       <c r="Q5" s="7">
-        <f>O5/P5</f>
+        <f t="shared" si="2"/>
         <v>0.32248974986485662</v>
       </c>
+      <c r="R5" s="5">
+        <v>9.6105913549299996E-2</v>
+      </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>25</v>
       </c>
@@ -936,11 +959,11 @@
         <v>42937</v>
       </c>
       <c r="K6" s="3">
-        <f>J6-5</f>
+        <f t="shared" si="0"/>
         <v>42932</v>
       </c>
       <c r="L6" s="3">
-        <f>J6</f>
+        <f t="shared" si="1"/>
         <v>42937</v>
       </c>
       <c r="M6" s="6">
@@ -956,11 +979,14 @@
         <v>190068280</v>
       </c>
       <c r="Q6" s="7">
-        <f>O6/P6</f>
+        <f t="shared" si="2"/>
         <v>0.52612671614642903</v>
       </c>
+      <c r="R6" s="5">
+        <v>9.92528586376E-2</v>
+      </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>20</v>
       </c>
@@ -984,11 +1010,11 @@
         <v>43056</v>
       </c>
       <c r="K7" s="3">
-        <f>J7-5</f>
+        <f t="shared" si="0"/>
         <v>43051</v>
       </c>
       <c r="L7" s="3">
-        <f>J7</f>
+        <f t="shared" si="1"/>
         <v>43056</v>
       </c>
       <c r="M7" s="6">
@@ -1004,11 +1030,14 @@
         <v>229024295</v>
       </c>
       <c r="Q7" s="7">
-        <f>O7/P7</f>
+        <f t="shared" si="2"/>
         <v>1.309904698102007</v>
       </c>
+      <c r="R7" s="5">
+        <v>9.2402942125600004E-2</v>
+      </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>26</v>
       </c>
@@ -1032,11 +1061,11 @@
         <v>42811</v>
       </c>
       <c r="K8" s="3">
-        <f>J8-5</f>
+        <f t="shared" si="0"/>
         <v>42806</v>
       </c>
       <c r="L8" s="3">
-        <f>J8</f>
+        <f t="shared" si="1"/>
         <v>42811</v>
       </c>
       <c r="M8" s="6">
@@ -1052,11 +1081,14 @@
         <v>504014165</v>
       </c>
       <c r="Q8" s="7">
-        <f>O8/P8</f>
+        <f t="shared" si="2"/>
         <v>0.31745139543845957</v>
       </c>
+      <c r="R8" s="5">
+        <v>0.14892632265700001</v>
+      </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
@@ -1080,11 +1112,11 @@
         <v>43014</v>
       </c>
       <c r="K9" s="3">
-        <f>J9-5</f>
+        <f t="shared" si="0"/>
         <v>43009</v>
       </c>
       <c r="L9" s="3">
-        <f>J9</f>
+        <f t="shared" si="1"/>
         <v>43014</v>
       </c>
       <c r="M9" s="6">
@@ -1100,11 +1132,14 @@
         <v>92054159</v>
       </c>
       <c r="Q9" s="7">
-        <f>O9/P9</f>
+        <f t="shared" si="2"/>
         <v>1.6837913863294325</v>
       </c>
+      <c r="R9" s="5">
+        <v>0.118894264242</v>
+      </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>21</v>
       </c>
@@ -1128,11 +1163,11 @@
         <v>43042</v>
       </c>
       <c r="K10" s="3">
-        <f>J10-5</f>
+        <f t="shared" si="0"/>
         <v>43037</v>
       </c>
       <c r="L10" s="3">
-        <f>J10</f>
+        <f t="shared" si="1"/>
         <v>43042</v>
       </c>
       <c r="M10" s="6">
@@ -1148,11 +1183,14 @@
         <v>315058289</v>
       </c>
       <c r="Q10" s="7">
-        <f>O10/P10</f>
+        <f t="shared" si="2"/>
         <v>0.57132285130895255</v>
       </c>
+      <c r="R10" s="5">
+        <v>8.10604753697E-2</v>
+      </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>15</v>
       </c>
@@ -1176,11 +1214,11 @@
         <v>42937</v>
       </c>
       <c r="K11" s="3">
-        <f>J11-5</f>
+        <f t="shared" si="0"/>
         <v>42932</v>
       </c>
       <c r="L11" s="3">
-        <f>J11</f>
+        <f t="shared" si="1"/>
         <v>42937</v>
       </c>
       <c r="M11" s="6">
@@ -1196,11 +1234,14 @@
         <v>389813101</v>
       </c>
       <c r="Q11" s="7">
-        <f>O11/P11</f>
+        <f t="shared" si="2"/>
         <v>0.51306638870508359</v>
       </c>
+      <c r="R11" s="5">
+        <v>0.148720333191</v>
+      </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
@@ -1224,11 +1265,11 @@
         <v>42776</v>
       </c>
       <c r="K12" s="3">
-        <f>J12-5</f>
+        <f t="shared" si="0"/>
         <v>42771</v>
       </c>
       <c r="L12" s="3">
-        <f>J12</f>
+        <f t="shared" si="1"/>
         <v>42776</v>
       </c>
       <c r="M12" s="6">
@@ -1244,11 +1285,14 @@
         <v>175750384</v>
       </c>
       <c r="Q12" s="7">
-        <f>O12/P12</f>
+        <f t="shared" si="2"/>
         <v>0.45519103958259344</v>
       </c>
+      <c r="R12" s="5">
+        <v>0.16990544716600001</v>
+      </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>16</v>
       </c>
@@ -1272,11 +1316,11 @@
         <v>42930</v>
       </c>
       <c r="K13" s="3">
-        <f>J13-5</f>
+        <f t="shared" si="0"/>
         <v>42925</v>
       </c>
       <c r="L13" s="3">
-        <f>J13</f>
+        <f t="shared" si="1"/>
         <v>42930</v>
       </c>
       <c r="M13" s="6">
@@ -1292,11 +1336,14 @@
         <v>146880162</v>
       </c>
       <c r="Q13" s="7">
-        <f>O13/P13</f>
+        <f t="shared" si="2"/>
         <v>1.0212407036969362</v>
       </c>
+      <c r="R13" s="5">
+        <v>9.4087649487499994E-2</v>
+      </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>23</v>
       </c>
@@ -1320,11 +1367,11 @@
         <v>43070</v>
       </c>
       <c r="K14" s="3">
-        <f>J14-5</f>
+        <f t="shared" si="0"/>
         <v>43065</v>
       </c>
       <c r="L14" s="3">
-        <f>J14</f>
+        <f t="shared" si="1"/>
         <v>43070</v>
       </c>
       <c r="M14" s="6">
@@ -1340,11 +1387,14 @@
         <v>63780344</v>
       </c>
       <c r="Q14" s="7">
-        <f>O14/P14</f>
+        <f t="shared" si="2"/>
         <v>0.30573682700739274</v>
       </c>
+      <c r="R14" s="5">
+        <v>0.112327180368</v>
+      </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>24</v>
       </c>
@@ -1368,11 +1418,11 @@
         <v>42880</v>
       </c>
       <c r="K15" s="3">
-        <f>J15-5</f>
+        <f t="shared" si="0"/>
         <v>42875</v>
       </c>
       <c r="L15" s="3">
-        <f>J15</f>
+        <f t="shared" si="1"/>
         <v>42880</v>
       </c>
       <c r="M15" s="6">
@@ -1388,11 +1438,14 @@
         <v>58060186</v>
       </c>
       <c r="Q15" s="7">
-        <f>O15/P15</f>
+        <f t="shared" si="2"/>
         <v>1.1884219592407093</v>
       </c>
+      <c r="R15" s="5">
+        <v>7.4725890321700003E-2</v>
+      </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>28</v>
       </c>
@@ -1416,11 +1469,11 @@
         <v>42863</v>
       </c>
       <c r="K16" s="3">
-        <f>J16-5</f>
+        <f t="shared" si="0"/>
         <v>42858</v>
       </c>
       <c r="L16" s="3">
-        <f>J16</f>
+        <f t="shared" si="1"/>
         <v>42863</v>
       </c>
       <c r="M16" s="6">
@@ -1436,8 +1489,11 @@
         <v>39175066</v>
       </c>
       <c r="Q16" s="7">
-        <f>O16/P16</f>
+        <f t="shared" si="2"/>
         <v>4.4671271262184984</v>
+      </c>
+      <c r="R16" s="5">
+        <v>0.138129282178</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added positive negative and neutral
</commit_message>
<xml_diff>
--- a/Data_Report.xlsx
+++ b/Data_Report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Shawn/CS491-BoxOffice/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DE588CB-63BF-6648-90EB-31FA658BEF72}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{233D6BC4-2C12-9647-8E50-C6046AF79ED8}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="13620" windowHeight="14340" xr2:uid="{B4E7339E-50A7-7345-85C7-648E0B2AFFAF}"/>
   </bookViews>
@@ -664,8 +664,8 @@
   <dimension ref="A1:R16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="Q1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="R16" sqref="R16"/>
+      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -751,6 +751,15 @@
         <f>SUM(Table2[[#This Row],[Total Tweets]:[Replies]])</f>
         <v>3428520</v>
       </c>
+      <c r="G2">
+        <v>60232</v>
+      </c>
+      <c r="H2">
+        <v>29703</v>
+      </c>
+      <c r="I2">
+        <v>56955</v>
+      </c>
       <c r="J2" s="3">
         <v>42790</v>
       </c>
@@ -802,6 +811,15 @@
         <f>SUM(Table2[[#This Row],[Total Tweets]:[Replies]])</f>
         <v>3160314</v>
       </c>
+      <c r="G3">
+        <v>58112</v>
+      </c>
+      <c r="H3">
+        <v>83316</v>
+      </c>
+      <c r="I3">
+        <v>26402</v>
+      </c>
       <c r="J3" s="3">
         <v>43147</v>
       </c>
@@ -853,6 +871,15 @@
         <f>SUM(Table2[[#This Row],[Total Tweets]:[Replies]])</f>
         <v>2345519</v>
       </c>
+      <c r="G4">
+        <v>67037</v>
+      </c>
+      <c r="H4">
+        <v>16596</v>
+      </c>
+      <c r="I4">
+        <v>122824</v>
+      </c>
       <c r="J4" s="3">
         <v>42888</v>
       </c>
@@ -904,6 +931,15 @@
         <f>SUM(Table2[[#This Row],[Total Tweets]:[Replies]])</f>
         <v>2236802</v>
       </c>
+      <c r="G5">
+        <v>48126</v>
+      </c>
+      <c r="H5">
+        <v>10434</v>
+      </c>
+      <c r="I5">
+        <v>58383</v>
+      </c>
       <c r="J5" s="3">
         <v>43084</v>
       </c>
@@ -955,6 +991,15 @@
         <f>SUM(Table2[[#This Row],[Total Tweets]:[Replies]])</f>
         <v>2163929</v>
       </c>
+      <c r="G6">
+        <v>38070</v>
+      </c>
+      <c r="H6">
+        <v>9163</v>
+      </c>
+      <c r="I6">
+        <v>73528</v>
+      </c>
       <c r="J6" s="3">
         <v>42937</v>
       </c>
@@ -1006,6 +1051,15 @@
         <f>SUM(Table2[[#This Row],[Total Tweets]:[Replies]])</f>
         <v>1867263</v>
       </c>
+      <c r="G7">
+        <v>59583</v>
+      </c>
+      <c r="H7">
+        <v>17456</v>
+      </c>
+      <c r="I7">
+        <v>109801</v>
+      </c>
       <c r="J7" s="3">
         <v>43056</v>
       </c>
@@ -1057,6 +1111,15 @@
         <f>SUM(Table2[[#This Row],[Total Tweets]:[Replies]])</f>
         <v>1323036</v>
       </c>
+      <c r="G8">
+        <v>44821</v>
+      </c>
+      <c r="H8">
+        <v>7417</v>
+      </c>
+      <c r="I8">
+        <v>60184</v>
+      </c>
       <c r="J8" s="3">
         <v>42811</v>
       </c>
@@ -1108,6 +1171,15 @@
         <f>SUM(Table2[[#This Row],[Total Tweets]:[Replies]])</f>
         <v>567214</v>
       </c>
+      <c r="G9">
+        <v>23968</v>
+      </c>
+      <c r="H9">
+        <v>4762</v>
+      </c>
+      <c r="I9">
+        <v>42884</v>
+      </c>
       <c r="J9" s="3">
         <v>43014</v>
       </c>
@@ -1159,6 +1231,15 @@
         <f>SUM(Table2[[#This Row],[Total Tweets]:[Replies]])</f>
         <v>565451</v>
       </c>
+      <c r="G10">
+        <v>30982</v>
+      </c>
+      <c r="H10">
+        <v>8036</v>
+      </c>
+      <c r="I10">
+        <v>85365</v>
+      </c>
       <c r="J10" s="3">
         <v>43042</v>
       </c>
@@ -1210,6 +1291,15 @@
         <f>SUM(Table2[[#This Row],[Total Tweets]:[Replies]])</f>
         <v>273095</v>
       </c>
+      <c r="G11">
+        <v>22707</v>
+      </c>
+      <c r="H11">
+        <v>3498</v>
+      </c>
+      <c r="I11">
+        <v>36183</v>
+      </c>
       <c r="J11" s="3">
         <v>42937</v>
       </c>
@@ -1261,6 +1351,15 @@
         <f>SUM(Table2[[#This Row],[Total Tweets]:[Replies]])</f>
         <v>151581</v>
       </c>
+      <c r="G12">
+        <v>12572</v>
+      </c>
+      <c r="H12">
+        <v>2061</v>
+      </c>
+      <c r="I12">
+        <v>18354</v>
+      </c>
       <c r="J12" s="3">
         <v>42776</v>
       </c>
@@ -1312,6 +1411,15 @@
         <f>SUM(Table2[[#This Row],[Total Tweets]:[Replies]])</f>
         <v>130388</v>
       </c>
+      <c r="G13">
+        <v>8751</v>
+      </c>
+      <c r="H13">
+        <v>3268</v>
+      </c>
+      <c r="I13">
+        <v>10782</v>
+      </c>
       <c r="J13" s="3">
         <v>42930</v>
       </c>
@@ -1363,6 +1471,15 @@
         <f>SUM(Table2[[#This Row],[Total Tweets]:[Replies]])</f>
         <v>104269</v>
       </c>
+      <c r="G14">
+        <v>4600</v>
+      </c>
+      <c r="H14">
+        <v>1373</v>
+      </c>
+      <c r="I14">
+        <v>4268</v>
+      </c>
       <c r="J14" s="3">
         <v>43070</v>
       </c>
@@ -1414,6 +1531,15 @@
         <f>SUM(Table2[[#This Row],[Total Tweets]:[Replies]])</f>
         <v>88344</v>
       </c>
+      <c r="G15">
+        <v>2385</v>
+      </c>
+      <c r="H15">
+        <v>690</v>
+      </c>
+      <c r="I15">
+        <v>4560</v>
+      </c>
       <c r="J15" s="3">
         <v>42880</v>
       </c>
@@ -1464,6 +1590,15 @@
       <c r="F16" s="5">
         <f>SUM(Table2[[#This Row],[Total Tweets]:[Replies]])</f>
         <v>32438</v>
+      </c>
+      <c r="G16">
+        <v>2275</v>
+      </c>
+      <c r="H16">
+        <v>484</v>
+      </c>
+      <c r="I16">
+        <v>3454</v>
       </c>
       <c r="J16" s="3">
         <v>42863</v>

</xml_diff>

<commit_message>
Added more charts and trendlines
</commit_message>
<xml_diff>
--- a/Data_Report.xlsx
+++ b/Data_Report.xlsx
@@ -8,17 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Logan/Documents/GitHub/CS491-BoxOffice/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{451EC455-9270-BD4D-BCB3-BCAF12A9E61A}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C33FA1DE-EB0D-8946-8846-9F9252E0AE38}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="24740" windowHeight="14340" xr2:uid="{B4E7339E-50A7-7345-85C7-648E0B2AFFAF}"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="41480" windowHeight="28340" xr2:uid="{B4E7339E-50A7-7345-85C7-648E0B2AFFAF}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
-    <sheet name="Positive vs Earnings" sheetId="14" r:id="rId2"/>
-    <sheet name="Tweets vs Ratio" sheetId="9" r:id="rId3"/>
-    <sheet name="Attention vs Ratio" sheetId="13" r:id="rId4"/>
-    <sheet name="Tweets vs Earnings" sheetId="4" r:id="rId5"/>
-    <sheet name="Attention vs Earnings" sheetId="5" r:id="rId6"/>
+    <sheet name="IMBD vs Positive" sheetId="15" r:id="rId2"/>
+    <sheet name="IMDB vs Tweets" sheetId="16" r:id="rId3"/>
+    <sheet name="Rotten vs Positive" sheetId="17" r:id="rId4"/>
+    <sheet name="Rotten vs Tweets" sheetId="18" r:id="rId5"/>
+    <sheet name="Positive vs Earnings" sheetId="14" r:id="rId6"/>
+    <sheet name="Tweets vs Ratio" sheetId="9" r:id="rId7"/>
+    <sheet name="Attention vs Ratio" sheetId="13" r:id="rId8"/>
+    <sheet name="Tweets vs Earnings" sheetId="4" r:id="rId9"/>
+    <sheet name="Attention vs Earnings" sheetId="5" r:id="rId10"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -216,10 +220,6 @@
   </cellStyles>
   <dxfs count="17">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -252,6 +252,10 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="m/d/yyyy;@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -346,6 +350,1709 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>IMDB vs Positive</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$M$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>IMDB</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Data!$G$2:$G$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>60232</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>58112</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>67037</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>48126</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>38070</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>59583</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44821</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>23968</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>30982</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>22707</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12572</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>8751</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4600</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2385</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2275</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Data!$M$2:$M$16</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>0.77</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.77</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.74</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.67</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.72</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.81</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.79</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.77</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.73</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.56000000000000005</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.68</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-AA1F-B549-8C47-DF210A422E6A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="348611760"/>
+        <c:axId val="348588432"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="348611760"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="348588432"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="348588432"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="348611760"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>IMDB vs Tweets</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$M$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>IMDB</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Data!$B$2:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>146890</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>167830</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>206457</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>116943</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>120761</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>186840</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>112422</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>71614</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>124383</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>62388</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>32987</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>22801</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>10241</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7365</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6212</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Data!$M$2:$M$16</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>0.77</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.77</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.74</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.67</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.72</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.81</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.79</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.77</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.73</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.56000000000000005</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.68</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-FAA9-4246-98D0-A14C085C7DC9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="389148320"/>
+        <c:axId val="389150016"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="389148320"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="389150016"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="389150016"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="389148320"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Rotten Tomatoes vs Positive</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$N$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Rotten Tomatoes</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:forward val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Data!$G$2:$G$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>60232</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>58112</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>67037</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>48126</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>38070</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>59583</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44821</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>23968</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>30982</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>22707</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12572</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>8751</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4600</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2385</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2275</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Data!$N$2:$N$16</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.97</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.92</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.91</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.92</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.71</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.87</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.92</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.93</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.92</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.18</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-EF07-EF49-A93A-42B49E2F941F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="386966704"/>
+        <c:axId val="386968400"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="386966704"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="386968400"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="386968400"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="386966704"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Rotten Tomatoes vs Total Tweets</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$N$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Rotten Tomatoes</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Data!$B$2:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>146890</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>167830</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>206457</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>116943</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>120761</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>186840</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>112422</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>71614</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>124383</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>62388</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>32987</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>22801</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>10241</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7365</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6212</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Data!$N$2:$N$16</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.97</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.92</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.91</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.92</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.71</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.87</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.92</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.93</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.92</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.18</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-2BA3-5C4D-A2D4-2B4D22925574}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="403075712"/>
+        <c:axId val="403382960"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="403075712"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="403382960"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="403382960"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="403075712"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -417,6 +2124,35 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:forward val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Data!$G$2:$G$16</c:f>
@@ -714,7 +2450,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -729,6 +2465,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Tweets vs Ratio</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -800,6 +2561,20 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Data!$B$2:$B$16</c:f>
@@ -1097,7 +2872,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1183,6 +2958,20 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Data!$F$2:$F$16</c:f>
@@ -1480,7 +3269,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1566,6 +3355,20 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Data!$B$2:$B$16</c:f>
@@ -1856,7 +3659,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1942,6 +3745,20 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Data!$F$2:$F$16</c:f>
@@ -2439,6 +4256,166 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors9.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -5019,11 +6996,2075 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style9.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{CF82584A-448C-FA45-A0E7-DFADCDDCBB06}">
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{9138307E-3317-0442-8ABC-3820C6D8031C}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="103" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="242" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5031,10 +9072,10 @@
 </file>
 
 <file path=xl/chartsheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{A9E3A668-D316-D441-9E14-27D2668AD2AB}">
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{F8245B89-D3CE-F94E-A34C-82BA8A03E4E8}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="103" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="242" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5042,10 +9083,10 @@
 </file>
 
 <file path=xl/chartsheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{14E527E0-748D-C842-B8C1-19005CE4A64D}">
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{B1F14764-3009-1744-A713-E4BEB7C73EE8}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="103" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="242" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5053,10 +9094,10 @@
 </file>
 
 <file path=xl/chartsheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{950E5C96-935D-A242-B8C9-33F87771D6BD}">
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{CA778CF7-2F0D-5B42-BC8C-CEAB934B1E62}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="103" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="242" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5064,10 +9105,54 @@
 </file>
 
 <file path=xl/chartsheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{CF82584A-448C-FA45-A0E7-DFADCDDCBB06}">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="242" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{A9E3A668-D316-D441-9E14-27D2668AD2AB}">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="242" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{14E527E0-748D-C842-B8C1-19005CE4A64D}">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="242" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{950E5C96-935D-A242-B8C9-33F87771D6BD}">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="242" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{F992D237-7F40-914F-B761-DA86F2D713F6}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="103" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="242" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5078,7 +9163,139 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8680388" cy="6288350"/>
+    <xdr:ext cx="8669587" cy="6281777"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5A24388C-F0B2-B847-9AD1-4E5801F4E8A9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8669587" cy="6281777"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D7421262-AC74-E946-ABB1-15D51BBBABAE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8669587" cy="6281777"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4D9AB950-1E78-5F41-86A9-E012510506A9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8669587" cy="6281777"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9BA51CAB-730A-7B4B-8D90-01D2B83A3A6E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8669587" cy="6281777"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -5107,11 +9324,11 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8680388" cy="6288350"/>
+    <xdr:ext cx="8669587" cy="6281777"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -5140,11 +9357,11 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8680388" cy="6288350"/>
+    <xdr:ext cx="8669587" cy="6281777"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -5173,11 +9390,11 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8680388" cy="6288350"/>
+    <xdr:ext cx="8669587" cy="6281777"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -5206,11 +9423,11 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8680388" cy="6288350"/>
+    <xdr:ext cx="8669587" cy="6281777"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -5251,27 +9468,27 @@
     <tableColumn id="3" xr3:uid="{92C49452-8A3A-8842-8631-089B162924F0}" name="Likes" dataDxfId="12"/>
     <tableColumn id="4" xr3:uid="{AD276103-5716-3B43-B6C8-8D949AA97202}" name="Retweets" dataDxfId="11"/>
     <tableColumn id="5" xr3:uid="{AA75EECD-212D-BD41-9C48-C3C1A08F0941}" name="Replies" dataDxfId="10"/>
-    <tableColumn id="18" xr3:uid="{76B65A6B-8381-9442-8554-32B37C575EB5}" name="Total Attention" dataDxfId="0">
+    <tableColumn id="18" xr3:uid="{76B65A6B-8381-9442-8554-32B37C575EB5}" name="Total Attention" dataDxfId="9">
       <calculatedColumnFormula>SUM(Table2[[#This Row],[Likes]:[Replies]])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{9223458C-5ED8-3849-AA94-94576A5BF092}" name="Positive"/>
     <tableColumn id="7" xr3:uid="{DEF0B644-D2D5-1E40-834A-4535773A529A}" name="Negative"/>
     <tableColumn id="8" xr3:uid="{A82D5766-72E4-0441-B63C-DF714B35673A}" name="Neutral"/>
-    <tableColumn id="9" xr3:uid="{E745E2B8-7D49-A040-8802-3CEDBEB430DF}" name="Release Date" dataDxfId="9"/>
-    <tableColumn id="10" xr3:uid="{F67DD7E8-AB5C-824C-8812-42D2B8DC891F}" name="Data Scrape Start" dataDxfId="8">
+    <tableColumn id="9" xr3:uid="{E745E2B8-7D49-A040-8802-3CEDBEB430DF}" name="Release Date" dataDxfId="8"/>
+    <tableColumn id="10" xr3:uid="{F67DD7E8-AB5C-824C-8812-42D2B8DC891F}" name="Data Scrape Start" dataDxfId="7">
       <calculatedColumnFormula>J2-5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{BFB3861C-0060-4D4E-B8CE-ADE8871979F4}" name="Data Scrape End" dataDxfId="7">
+    <tableColumn id="11" xr3:uid="{BFB3861C-0060-4D4E-B8CE-ADE8871979F4}" name="Data Scrape End" dataDxfId="6">
       <calculatedColumnFormula>J2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{B8018AB7-FF15-C04A-A4DB-8C4612CED9D9}" name="IMDB" dataDxfId="6"/>
-    <tableColumn id="13" xr3:uid="{9BBFE118-814E-F343-A9AC-AB50B6206221}" name="Rotten Tomatoes" dataDxfId="5"/>
-    <tableColumn id="14" xr3:uid="{936BFE96-DD47-9B4D-9367-1EE99BB5465A}" name="Movie Budget" dataDxfId="4"/>
-    <tableColumn id="15" xr3:uid="{E83FF061-27B7-C84E-8DFD-65091A59DDE5}" name="Movie Earnings" dataDxfId="3"/>
-    <tableColumn id="16" xr3:uid="{6F8934A3-5EF3-A54E-B767-90F815BBFDC5}" name="Ratio" dataDxfId="2">
+    <tableColumn id="12" xr3:uid="{B8018AB7-FF15-C04A-A4DB-8C4612CED9D9}" name="IMDB" dataDxfId="5"/>
+    <tableColumn id="13" xr3:uid="{9BBFE118-814E-F343-A9AC-AB50B6206221}" name="Rotten Tomatoes" dataDxfId="4"/>
+    <tableColumn id="14" xr3:uid="{936BFE96-DD47-9B4D-9367-1EE99BB5465A}" name="Movie Budget" dataDxfId="3"/>
+    <tableColumn id="15" xr3:uid="{E83FF061-27B7-C84E-8DFD-65091A59DDE5}" name="Movie Earnings" dataDxfId="2"/>
+    <tableColumn id="16" xr3:uid="{6F8934A3-5EF3-A54E-B767-90F815BBFDC5}" name="Ratio" dataDxfId="1">
       <calculatedColumnFormula>O2/P2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{67442503-5FA6-7243-86D7-290816640E7A}" name="Sentiment Analysis" dataDxfId="1"/>
+    <tableColumn id="17" xr3:uid="{67442503-5FA6-7243-86D7-290816640E7A}" name="Sentiment Analysis" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5578,7 +9795,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C18" sqref="C18"/>
+      <selection pane="topRight" activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>